<commit_message>
Adjust pjm5bus case line rate_a
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_demo.xlsx
+++ b/ams/cases/5bus/pjm5bus_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350B2381-DDFA-F541-83C8-A9D296ED9066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DC8413-5FD9-9840-91E4-832A1F036AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="7420" windowWidth="21600" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -1722,7 +1722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2777B7D7-CE5C-114E-9B38-A548A06A92E7}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -3007,9 +3007,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView zoomScale="165" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="165" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3212,7 +3212,7 @@
         <v>6.5799999999999999E-3</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -3286,7 +3286,7 @@
         <v>3.1260000000000003E-2</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -3360,7 +3360,7 @@
         <v>1.8519999999999998E-2</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -3434,7 +3434,7 @@
         <v>6.7400000000000003E-3</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O6">
         <v>0</v>

</xml_diff>

<commit_message>
Rename model Region to Zone for clarity
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_demo.xlsx
+++ b/ams/cases/5bus/pjm5bus_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85DF813-9AF0-494B-A23D-CBAD2F212365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9A681A-257B-8941-B2F3-8C8759A4DA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="700" windowWidth="21600" windowHeight="18940" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="700" windowWidth="21600" windowHeight="18940" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="GCost" sheetId="11" r:id="rId7"/>
     <sheet name="Line" sheetId="5" r:id="rId8"/>
     <sheet name="Area" sheetId="6" r:id="rId9"/>
-    <sheet name="Region" sheetId="10" r:id="rId10"/>
+    <sheet name="Zone" sheetId="10" r:id="rId10"/>
     <sheet name="EDTSlot" sheetId="12" r:id="rId11"/>
     <sheet name="UCTSlot" sheetId="13" r:id="rId12"/>
     <sheet name="SFR" sheetId="15" r:id="rId13"/>
@@ -1279,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB94B98-B38A-EC46-833E-965628D04701}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3624,7 +3624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>

</xml_diff>

<commit_message>
Update case pjm5bus_demo for testing purpose
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_demo.xlsx
+++ b/ams/cases/5bus/pjm5bus_demo.xlsx
@@ -8,30 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9A681A-257B-8941-B2F3-8C8759A4DA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3443BA-A5C2-DC40-B6BD-8BA097E4E790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="700" windowWidth="21600" windowHeight="18940" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
     <sheet name="Bus" sheetId="1" r:id="rId2"/>
-    <sheet name="PQ" sheetId="2" r:id="rId3"/>
-    <sheet name="PV" sheetId="3" r:id="rId4"/>
-    <sheet name="ESD1" sheetId="22" r:id="rId5"/>
-    <sheet name="Slack" sheetId="4" r:id="rId6"/>
-    <sheet name="GCost" sheetId="11" r:id="rId7"/>
-    <sheet name="Line" sheetId="5" r:id="rId8"/>
-    <sheet name="Area" sheetId="6" r:id="rId9"/>
-    <sheet name="Zone" sheetId="10" r:id="rId10"/>
-    <sheet name="EDTSlot" sheetId="12" r:id="rId11"/>
-    <sheet name="UCTSlot" sheetId="13" r:id="rId12"/>
-    <sheet name="SFR" sheetId="15" r:id="rId13"/>
-    <sheet name="SFRCost" sheetId="16" r:id="rId14"/>
-    <sheet name="SR" sheetId="17" r:id="rId15"/>
-    <sheet name="SRCost" sheetId="18" r:id="rId16"/>
-    <sheet name="NSR" sheetId="19" r:id="rId17"/>
-    <sheet name="NSRCost" sheetId="20" r:id="rId18"/>
-    <sheet name="DCost" sheetId="23" r:id="rId19"/>
+    <sheet name="VSGR" sheetId="25" r:id="rId3"/>
+    <sheet name="VSGCost" sheetId="26" r:id="rId4"/>
+    <sheet name="REGCV1" sheetId="24" r:id="rId5"/>
+    <sheet name="PQ" sheetId="2" r:id="rId6"/>
+    <sheet name="PV" sheetId="3" r:id="rId7"/>
+    <sheet name="ESD1" sheetId="22" r:id="rId8"/>
+    <sheet name="Slack" sheetId="4" r:id="rId9"/>
+    <sheet name="GCost" sheetId="11" r:id="rId10"/>
+    <sheet name="Line" sheetId="5" r:id="rId11"/>
+    <sheet name="Area" sheetId="6" r:id="rId12"/>
+    <sheet name="Zone" sheetId="10" r:id="rId13"/>
+    <sheet name="EDTSlot" sheetId="12" r:id="rId14"/>
+    <sheet name="UCTSlot" sheetId="13" r:id="rId15"/>
+    <sheet name="SFR" sheetId="15" r:id="rId16"/>
+    <sheet name="SFRCost" sheetId="16" r:id="rId17"/>
+    <sheet name="SR" sheetId="17" r:id="rId18"/>
+    <sheet name="SRCost" sheetId="18" r:id="rId19"/>
+    <sheet name="NSR" sheetId="19" r:id="rId20"/>
+    <sheet name="NSRCost" sheetId="20" r:id="rId21"/>
+    <sheet name="DCost" sheetId="23" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="204">
   <si>
     <t>idx</t>
   </si>
@@ -701,6 +704,84 @@
   </si>
   <si>
     <t>Line_7</t>
+  </si>
+  <si>
+    <t>Mmax</t>
+  </si>
+  <si>
+    <t>Dmax</t>
+  </si>
+  <si>
+    <t>gammap</t>
+  </si>
+  <si>
+    <t>gammaq</t>
+  </si>
+  <si>
+    <t>VSG_1</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>VSG_2</t>
+  </si>
+  <si>
+    <t>VSG_3</t>
+  </si>
+  <si>
+    <t>VSG_4</t>
+  </si>
+  <si>
+    <t>dvm</t>
+  </si>
+  <si>
+    <t>dvd</t>
+  </si>
+  <si>
+    <t>VSGR_1</t>
+  </si>
+  <si>
+    <t>VSGR 1</t>
+  </si>
+  <si>
+    <t>VSGR_2</t>
+  </si>
+  <si>
+    <t>VSGR 2</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>VSGCost_1</t>
+  </si>
+  <si>
+    <t>VSGCost 1</t>
+  </si>
+  <si>
+    <t>VSGCost_2</t>
+  </si>
+  <si>
+    <t>VSGCost 2</t>
+  </si>
+  <si>
+    <t>VSGCost_3</t>
+  </si>
+  <si>
+    <t>VSGCost 3</t>
+  </si>
+  <si>
+    <t>VSGCost_4</t>
+  </si>
+  <si>
+    <t>VSGCost 4</t>
   </si>
 </sst>
 </file>
@@ -1276,10 +1357,917 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0.3</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0.4</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0.1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.01</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AA8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <v>230</v>
+      </c>
+      <c r="J2">
+        <v>230</v>
+      </c>
+      <c r="K2">
+        <v>2.81E-3</v>
+      </c>
+      <c r="L2">
+        <v>2.81E-2</v>
+      </c>
+      <c r="M2">
+        <v>7.1199999999999996E-3</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <v>230</v>
+      </c>
+      <c r="J3">
+        <v>230</v>
+      </c>
+      <c r="K3">
+        <v>3.0400000000000002E-3</v>
+      </c>
+      <c r="L3">
+        <v>3.04E-2</v>
+      </c>
+      <c r="M3">
+        <v>6.5799999999999999E-3</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>230</v>
+      </c>
+      <c r="J4">
+        <v>230</v>
+      </c>
+      <c r="K4">
+        <v>6.4000000000000005E-4</v>
+      </c>
+      <c r="L4">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="M4">
+        <v>3.1260000000000003E-2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <v>230</v>
+      </c>
+      <c r="J5">
+        <v>230</v>
+      </c>
+      <c r="K5">
+        <v>1.08E-3</v>
+      </c>
+      <c r="L5">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="M5">
+        <v>1.8519999999999998E-2</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+      <c r="I6">
+        <v>230</v>
+      </c>
+      <c r="J6">
+        <v>230</v>
+      </c>
+      <c r="K6">
+        <v>2.97E-3</v>
+      </c>
+      <c r="L6">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="M6">
+        <v>6.7400000000000003E-3</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7">
+        <v>230</v>
+      </c>
+      <c r="J7">
+        <v>230</v>
+      </c>
+      <c r="K7">
+        <v>2.97E-3</v>
+      </c>
+      <c r="L7">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="M7">
+        <v>6.7400000000000003E-3</v>
+      </c>
+      <c r="N7">
+        <v>2.4</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>60</v>
+      </c>
+      <c r="I8">
+        <v>230</v>
+      </c>
+      <c r="J8">
+        <v>230</v>
+      </c>
+      <c r="K8">
+        <v>2.81E-3</v>
+      </c>
+      <c r="L8">
+        <v>2.81E-2</v>
+      </c>
+      <c r="M8">
+        <v>7.1199999999999996E-3</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB94B98-B38A-EC46-833E-965628D04701}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -1332,7 +2320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787DEB6E-5407-D64E-8FD6-1F71A62EBC04}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -1545,7 +2533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2777B7D7-CE5C-114E-9B38-A548A06A92E7}">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -1740,7 +2728,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0222B4-433A-4847-9EF9-ED7322586C33}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1824,7 +2812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369B7ED6-0339-A34F-8D4C-28B9C408DB19}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1942,7 +2930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BC4103-A416-3E41-9041-99544891E416}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2017,7 +3005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB172BE7-B3C0-A449-8F62-0781AC3DED02}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -2113,276 +3101,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145CFC81-A232-1D4D-AC9D-AC7308213471}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16">
-      <c r="A2" s="7">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF8DCDA-3E95-6745-801C-7005462F6D2D}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA5987A-571E-F945-B64B-3E7A6C256E6B}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="13">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="13">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="13">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2652,7 +3370,712 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145CFC81-A232-1D4D-AC9D-AC7308213471}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF8DCDA-3E95-6745-801C-7005462F6D2D}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA5987A-571E-F945-B64B-3E7A6C256E6B}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="13">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB7B987-34E2-6D4B-A577-F5965739C89F}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="4">
+        <v>532</v>
+      </c>
+      <c r="F2" s="4">
+        <v>78</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEC8492-2AAA-8647-BADE-3688636A5396}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600E4F84-EBED-D64A-A84B-ED12E42B5C88}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K1" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1" t="s">
+        <v>180</v>
+      </c>
+      <c r="M1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>143</v>
+      </c>
+      <c r="K2" s="3">
+        <v>23</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="H3" s="3">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>143</v>
+      </c>
+      <c r="K3" s="3">
+        <v>23</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="H4" s="3">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>143</v>
+      </c>
+      <c r="K4" s="3">
+        <v>23</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
+      <c r="H5" s="3">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>143</v>
+      </c>
+      <c r="K5" s="3">
+        <v>23</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -2812,13 +4235,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3144,7 +4567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD37CC2-7295-9745-AE86-E7562082AFC8}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -3241,7 +4664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V9"/>
   <sheetViews>
@@ -3392,911 +4815,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
-  <dimension ref="A1:K6"/>
-  <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0.3</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0.4</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0.1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0.01</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AA8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:27">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2">
-        <v>60</v>
-      </c>
-      <c r="I2">
-        <v>230</v>
-      </c>
-      <c r="J2">
-        <v>230</v>
-      </c>
-      <c r="K2">
-        <v>2.81E-3</v>
-      </c>
-      <c r="L2">
-        <v>2.81E-2</v>
-      </c>
-      <c r="M2">
-        <v>7.1199999999999996E-3</v>
-      </c>
-      <c r="N2">
-        <v>4</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
-        <v>60</v>
-      </c>
-      <c r="I3">
-        <v>230</v>
-      </c>
-      <c r="J3">
-        <v>230</v>
-      </c>
-      <c r="K3">
-        <v>3.0400000000000002E-3</v>
-      </c>
-      <c r="L3">
-        <v>3.04E-2</v>
-      </c>
-      <c r="M3">
-        <v>6.5799999999999999E-3</v>
-      </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <v>60</v>
-      </c>
-      <c r="I4">
-        <v>230</v>
-      </c>
-      <c r="J4">
-        <v>230</v>
-      </c>
-      <c r="K4">
-        <v>6.4000000000000005E-4</v>
-      </c>
-      <c r="L4">
-        <v>6.4000000000000003E-3</v>
-      </c>
-      <c r="M4">
-        <v>3.1260000000000003E-2</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5">
-        <v>60</v>
-      </c>
-      <c r="I5">
-        <v>230</v>
-      </c>
-      <c r="J5">
-        <v>230</v>
-      </c>
-      <c r="K5">
-        <v>1.08E-3</v>
-      </c>
-      <c r="L5">
-        <v>1.0800000000000001E-2</v>
-      </c>
-      <c r="M5">
-        <v>1.8519999999999998E-2</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-      <c r="H6">
-        <v>60</v>
-      </c>
-      <c r="I6">
-        <v>230</v>
-      </c>
-      <c r="J6">
-        <v>230</v>
-      </c>
-      <c r="K6">
-        <v>2.97E-3</v>
-      </c>
-      <c r="L6">
-        <v>2.9700000000000001E-2</v>
-      </c>
-      <c r="M6">
-        <v>6.7400000000000003E-3</v>
-      </c>
-      <c r="N6">
-        <v>2</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-      <c r="H7">
-        <v>60</v>
-      </c>
-      <c r="I7">
-        <v>230</v>
-      </c>
-      <c r="J7">
-        <v>230</v>
-      </c>
-      <c r="K7">
-        <v>2.97E-3</v>
-      </c>
-      <c r="L7">
-        <v>2.9700000000000001E-2</v>
-      </c>
-      <c r="M7">
-        <v>6.7400000000000003E-3</v>
-      </c>
-      <c r="N7">
-        <v>2.4</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>146</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-      <c r="H8">
-        <v>60</v>
-      </c>
-      <c r="I8">
-        <v>230</v>
-      </c>
-      <c r="J8">
-        <v>230</v>
-      </c>
-      <c r="K8">
-        <v>2.81E-3</v>
-      </c>
-      <c r="L8">
-        <v>2.81E-2</v>
-      </c>
-      <c r="M8">
-        <v>7.1199999999999996E-3</v>
-      </c>
-      <c r="N8">
-        <v>4</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>1</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Switch from zone to area in RTED
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_demo.xlsx
+++ b/ams/cases/5bus/pjm5bus_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3443BA-A5C2-DC40-B6BD-8BA097E4E790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED5A869-1259-3A47-9E8F-456614F83FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="215">
   <si>
     <t>idx</t>
   </si>
@@ -194,15 +194,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>ZONE_1</t>
-  </si>
-  <si>
-    <t>ZONE1</t>
-  </si>
-  <si>
-    <t>ZONE2</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -378,9 +369,6 @@
   </si>
   <si>
     <t>NSRC_4</t>
-  </si>
-  <si>
-    <t>ZONE_2</t>
   </si>
   <si>
     <t>field</t>
@@ -782,6 +770,51 @@
   </si>
   <si>
     <t>VSGCost 4</t>
+  </si>
+  <si>
+    <t>Zone_A</t>
+  </si>
+  <si>
+    <t>Zone_B</t>
+  </si>
+  <si>
+    <t>Zone_C</t>
+  </si>
+  <si>
+    <t>Zone_D</t>
+  </si>
+  <si>
+    <t>Zone_E</t>
+  </si>
+  <si>
+    <t>Zone A</t>
+  </si>
+  <si>
+    <t>Zone B</t>
+  </si>
+  <si>
+    <t>Zone C</t>
+  </si>
+  <si>
+    <t>Zone D</t>
+  </si>
+  <si>
+    <t>Zone E</t>
+  </si>
+  <si>
+    <t>SFR3</t>
+  </si>
+  <si>
+    <t>SR3</t>
+  </si>
+  <si>
+    <t>NSR3</t>
+  </si>
+  <si>
+    <t>VSGR_3</t>
+  </si>
+  <si>
+    <t>VSGR 3</t>
   </si>
 </sst>
 </file>
@@ -1315,16 +1348,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16">
@@ -1332,10 +1365,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -1345,10 +1378,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1383,22 +1416,22 @@
         <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1406,16 +1439,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1441,16 +1474,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1476,16 +1509,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1511,16 +1544,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1546,16 +1579,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -1634,13 +1667,13 @@
         <v>35</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>36</v>
@@ -1681,13 +1714,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1755,13 +1788,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1829,13 +1862,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1903,13 +1936,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1977,13 +2010,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2051,13 +2084,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -2125,13 +2158,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2265,10 +2298,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB94B98-B38A-EC46-833E-965628D04701}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2291,28 +2324,70 @@
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>46</v>
+      <c r="B2" t="s">
+        <v>200</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>47</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>108</v>
+      <c r="B3" t="s">
+        <v>201</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>48</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2341,95 +2416,95 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16">
       <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" t="s">
         <v>150</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E6" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16">
@@ -2554,77 +2629,77 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16">
@@ -2730,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0222B4-433A-4847-9EF9-ED7322586C33}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2752,13 +2827,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16">
@@ -2766,13 +2841,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E2" s="7">
         <v>0.03</v>
@@ -2780,8 +2855,8 @@
       <c r="F2" s="7">
         <v>0.03</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>47</v>
+      <c r="G2" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16">
@@ -2789,13 +2864,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E3" s="7">
         <v>0.03</v>
@@ -2803,11 +2878,35 @@
       <c r="F3" s="7">
         <v>0.03</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>48</v>
+      <c r="G3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2833,95 +2932,95 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
-        <v>72</v>
-      </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2932,10 +3031,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BC4103-A416-3E41-9041-99544891E416}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2954,10 +3053,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16">
@@ -2965,19 +3064,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E2" s="7">
         <v>0.03</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>47</v>
+      <c r="F2" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16">
@@ -2985,22 +3084,43 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E3" s="7">
         <v>0.03</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>48</v>
+      <c r="F3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3026,18 +3146,18 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3">
         <v>0.1</v>
@@ -3045,13 +3165,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3">
         <v>0.1</v>
@@ -3059,13 +3179,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D4" s="3">
         <v>0.1</v>
@@ -3073,13 +3193,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D5" s="3">
         <v>0.1</v>
@@ -3087,13 +3207,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D6" s="3">
         <v>0.1</v>
@@ -3111,7 +3231,7 @@
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3171,7 +3291,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <v>230</v>
@@ -3198,7 +3318,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>46</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3212,7 +3332,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E3">
         <v>230</v>
@@ -3239,7 +3359,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>46</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3253,7 +3373,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4">
         <v>230</v>
@@ -3280,7 +3400,7 @@
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3321,7 +3441,7 @@
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>46</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3335,7 +3455,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E6">
         <v>230</v>
@@ -3362,7 +3482,7 @@
         <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>46</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3372,10 +3492,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145CFC81-A232-1D4D-AC9D-AC7308213471}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3394,10 +3514,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16">
@@ -3405,19 +3525,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E2" s="7">
         <v>0.01</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>47</v>
+      <c r="F2" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16">
@@ -3425,22 +3545,43 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E3" s="7">
         <v>0.01</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>48</v>
+      <c r="F3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3466,18 +3607,18 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3">
         <v>0.1</v>
@@ -3485,13 +3626,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3">
         <v>0.1</v>
@@ -3499,13 +3640,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D4" s="3">
         <v>0.1</v>
@@ -3513,13 +3654,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D5" s="3">
         <v>0.1</v>
@@ -3527,13 +3668,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D6" s="3">
         <v>0.1</v>
@@ -3569,10 +3710,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3580,16 +3721,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F2" s="2">
         <v>1000</v>
@@ -3600,16 +3741,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F3" s="2">
         <v>1000</v>
@@ -3620,16 +3761,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F4" s="2">
         <v>1000</v>
@@ -3642,10 +3783,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB7B987-34E2-6D4B-A577-F5965739C89F}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3664,13 +3805,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3678,13 +3819,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4">
         <v>532</v>
@@ -3692,8 +3833,8 @@
       <c r="F2" s="4">
         <v>78</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>47</v>
+      <c r="G2" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3701,13 +3842,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E3" s="4">
         <v>0</v>
@@ -3715,11 +3856,35 @@
       <c r="F3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>48</v>
+      <c r="G3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3728,7 +3893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEC8492-2AAA-8647-BADE-3688636A5396}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
@@ -3748,13 +3913,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3762,16 +3927,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F2" s="2">
         <v>1.0000000000000001E-5</v>
@@ -3785,16 +3950,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F3" s="2">
         <v>2.0000000000000002E-5</v>
@@ -3808,16 +3973,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F4" s="2">
         <v>3.0000000000000001E-5</v>
@@ -3831,16 +3996,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F5" s="2">
         <v>4.0000000000000003E-5</v>
@@ -3887,22 +4052,22 @@
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I1" t="s">
         <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="L1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="M1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -3910,19 +4075,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E2" s="3">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G2">
         <v>200</v>
@@ -3951,19 +4116,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G3">
         <v>200</v>
@@ -3992,19 +4157,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G4">
         <v>200</v>
@@ -4033,19 +4198,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G5">
         <v>200</v>
@@ -4121,7 +4286,7 @@
         <v>12</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -4129,7 +4294,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4164,7 +4329,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -4199,7 +4364,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -4299,10 +4464,10 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -4318,13 +4483,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -4380,13 +4545,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -4442,13 +4607,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -4504,13 +4669,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -4579,43 +4744,43 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>134</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -4623,19 +4788,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C2" s="14">
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E2" s="14">
         <v>1</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G2" s="14">
         <v>100</v>
@@ -4728,10 +4893,10 @@
         <v>5</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>26</v>
@@ -4748,13 +4913,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E2">
         <v>100</v>

</xml_diff>

<commit_message>
Fix UC for swithcing from zone to area
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_demo.xlsx
+++ b/ams/cases/5bus/pjm5bus_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED5A869-1259-3A47-9E8F-456614F83FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9CC432-6621-6440-B12E-16B910A1B55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" firstSheet="5" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="214">
   <si>
     <t>idx</t>
   </si>
@@ -655,21 +655,9 @@
     <t>PJM 5-bus case for demo</t>
   </si>
   <si>
-    <t>0.9, 0</t>
-  </si>
-  <si>
-    <t>0.8, 0</t>
-  </si>
-  <si>
     <t>EDT5</t>
   </si>
   <si>
-    <t>1, 0</t>
-  </si>
-  <si>
-    <t>0.8, 1</t>
-  </si>
-  <si>
     <t>UCT5</t>
   </si>
   <si>
@@ -815,6 +803,15 @@
   </si>
   <si>
     <t>VSGR 3</t>
+  </si>
+  <si>
+    <t>0.8, 0.8, 0.8</t>
+  </si>
+  <si>
+    <t>0.9, 0.9, 0.9</t>
+  </si>
+  <si>
+    <t>1, 1, 1</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1788,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1862,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1936,7 +1933,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2010,7 +2007,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2084,7 +2081,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2158,7 +2155,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2239,7 +2236,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2268,6 +2265,9 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
@@ -2279,6 +2279,9 @@
       <c r="C3">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -2289,6 +2292,9 @@
       </c>
       <c r="C4">
         <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2325,13 +2331,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2339,13 +2345,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2353,13 +2359,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2367,13 +2373,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2381,13 +2387,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2433,7 +2439,7 @@
         <v>70</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="E2" t="s">
         <v>150</v>
@@ -2450,7 +2456,7 @@
         <v>72</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>161</v>
+        <v>212</v>
       </c>
       <c r="E3" t="s">
         <v>150</v>
@@ -2467,7 +2473,7 @@
         <v>74</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
         <v>150</v>
@@ -2484,7 +2490,7 @@
         <v>76</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>161</v>
+        <v>212</v>
       </c>
       <c r="E5" t="s">
         <v>150</v>
@@ -2495,13 +2501,13 @@
         <v>146</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
         <v>150</v>
@@ -2613,7 +2619,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2643,7 +2649,7 @@
         <v>77</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">
@@ -2657,7 +2663,7 @@
         <v>78</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>161</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16">
@@ -2671,7 +2677,7 @@
         <v>79</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16">
@@ -2685,7 +2691,7 @@
         <v>80</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>161</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16">
@@ -2693,13 +2699,13 @@
         <v>146</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16">
@@ -2887,13 +2893,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E4" s="7">
         <v>0.03</v>
@@ -3104,13 +3110,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E4" s="7">
         <v>0.03</v>
@@ -3231,7 +3237,7 @@
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2:M6"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3318,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3359,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3400,7 +3406,7 @@
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3441,7 +3447,7 @@
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3482,7 +3488,7 @@
         <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3495,7 +3501,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3554,7 +3560,7 @@
         <v>99</v>
       </c>
       <c r="E3" s="7">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F3" s="7">
         <v>2</v>
@@ -3565,16 +3571,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E4" s="7">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
         <v>3</v>
@@ -3805,10 +3811,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>10</v>
@@ -3819,13 +3825,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E2" s="4">
         <v>532</v>
@@ -3842,13 +3848,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E3" s="4">
         <v>0</v>
@@ -3865,13 +3871,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
@@ -3913,13 +3919,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3927,16 +3933,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F2" s="2">
         <v>1.0000000000000001E-5</v>
@@ -3950,16 +3956,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F3" s="2">
         <v>2.0000000000000002E-5</v>
@@ -3973,16 +3979,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F4" s="2">
         <v>3.0000000000000001E-5</v>
@@ -3996,16 +4002,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F5" s="2">
         <v>4.0000000000000003E-5</v>
@@ -4052,22 +4058,22 @@
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I1" t="s">
         <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="L1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="M1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -4075,13 +4081,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E2" s="3">
         <v>2</v>
@@ -4116,13 +4122,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -4157,13 +4163,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -4198,13 +4204,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>
@@ -4406,7 +4412,7 @@
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4737,7 +4743,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fix case pjm5bus_demo regarding ED and UC
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_demo.xlsx
+++ b/ams/cases/5bus/pjm5bus_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907446C9-8348-7E47-9051-4F1C9CE9C7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29C29C2-156B-2740-9BD4-FC4F1A9EFECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="293">
   <si>
     <t>idx</t>
   </si>
@@ -652,9 +652,6 @@
     <t>Dcost 3</t>
   </si>
   <si>
-    <t>PJM 5-bus case for demo</t>
-  </si>
-  <si>
     <t>EDT5</t>
   </si>
   <si>
@@ -805,13 +802,253 @@
     <t>VSGR 3</t>
   </si>
   <si>
-    <t>0.8, 0.8, 0.8</t>
-  </si>
-  <si>
-    <t>0.9, 0.9, 0.9</t>
-  </si>
-  <si>
     <t>1, 1, 1</t>
+  </si>
+  <si>
+    <t>0.793, 0.793, 0.793</t>
+  </si>
+  <si>
+    <t>0.756, 0.756, 0.756</t>
+  </si>
+  <si>
+    <t>0.723, 0.723, 0.723</t>
+  </si>
+  <si>
+    <t>0.708, 0.708, 0.708</t>
+  </si>
+  <si>
+    <t>0.706, 0.706, 0.706</t>
+  </si>
+  <si>
+    <t>0.75, 0.75, 0.75</t>
+  </si>
+  <si>
+    <t>0.802, 0.802, 0.802</t>
+  </si>
+  <si>
+    <t>0.828, 0.828, 0.828</t>
+  </si>
+  <si>
+    <t>0.851, 0.851, 0.851</t>
+  </si>
+  <si>
+    <t>0.874, 0.874, 0.874</t>
+  </si>
+  <si>
+    <t>0.898, 0.898, 0.898</t>
+  </si>
+  <si>
+    <t>0.919, 0.919, 0.919</t>
+  </si>
+  <si>
+    <t>0.947, 0.947, 0.947</t>
+  </si>
+  <si>
+    <t>0.97, 0.97, 0.97</t>
+  </si>
+  <si>
+    <t>0.987, 0.987, 0.987</t>
+  </si>
+  <si>
+    <t>0.991, 0.991, 0.991</t>
+  </si>
+  <si>
+    <t>0.956, 0.956, 0.956</t>
+  </si>
+  <si>
+    <t>0.93, 0.93, 0.93</t>
+  </si>
+  <si>
+    <t>0.905, 0.905, 0.905</t>
+  </si>
+  <si>
+    <t>0.849, 0.849, 0.849</t>
+  </si>
+  <si>
+    <t>0.784, 0.784, 0.784</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>EDT6</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>EDT7</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>EDT8</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>EDT9</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>EDT10</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>EDT11</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>EDT12</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>EDT13</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>EDT14</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>EDT15</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>EDT16</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>EDT17</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>EDT18</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>EDT19</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>EDT20</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>EDT21</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>EDT22</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>EDT23</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>EDT24</t>
+  </si>
+  <si>
+    <t>UCT6</t>
+  </si>
+  <si>
+    <t>UCT7</t>
+  </si>
+  <si>
+    <t>UCT8</t>
+  </si>
+  <si>
+    <t>UCT9</t>
+  </si>
+  <si>
+    <t>UCT10</t>
+  </si>
+  <si>
+    <t>UCT11</t>
+  </si>
+  <si>
+    <t>UCT12</t>
+  </si>
+  <si>
+    <t>UCT13</t>
+  </si>
+  <si>
+    <t>UCT14</t>
+  </si>
+  <si>
+    <t>UCT15</t>
+  </si>
+  <si>
+    <t>UCT16</t>
+  </si>
+  <si>
+    <t>UCT17</t>
+  </si>
+  <si>
+    <t>UCT18</t>
+  </si>
+  <si>
+    <t>UCT19</t>
+  </si>
+  <si>
+    <t>UCT20</t>
+  </si>
+  <si>
+    <t>UCT21</t>
+  </si>
+  <si>
+    <t>UCT22</t>
+  </si>
+  <si>
+    <t>UCT23</t>
+  </si>
+  <si>
+    <t>UCT24</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Load factor in EDTSlot and UCTSlot sourced from PJM 5-minutes load on August 30, 2023</t>
+  </si>
+  <si>
+    <t>PJM 5-bus case for demo purpose</t>
+  </si>
+  <si>
+    <t>0.7, 0.7, 0.7</t>
   </si>
 </sst>
 </file>
@@ -1332,15 +1569,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61E0E47-E5E8-FA43-A027-51A5C4ADA178}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1357,7 +1594,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:8" ht="16">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1365,19 +1602,35 @@
         <v>109</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>160</v>
+        <v>291</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>110</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1616,7 +1869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R31" sqref="R31"/>
     </sheetView>
@@ -1711,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1785,7 +2038,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1859,7 +2112,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1933,7 +2186,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2007,7 +2260,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2081,7 +2334,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2155,7 +2408,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2331,13 +2584,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2345,13 +2598,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2359,13 +2612,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2373,13 +2626,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2387,13 +2640,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2405,11 +2658,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787DEB6E-5407-D64E-8FD6-1F71A62EBC04}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16">
       <c r="A1" t="s">
@@ -2490,7 +2746,7 @@
         <v>76</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E5" t="s">
         <v>150</v>
@@ -2501,112 +2757,340 @@
         <v>146</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>211</v>
+        <v>292</v>
       </c>
       <c r="E6" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
+      <c r="A7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="16">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
+      <c r="A8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="16">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
+      <c r="A9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="16">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
+      <c r="A10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="16">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
+      <c r="A11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="16">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="A12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E12" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="16">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
+      <c r="A13" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E13" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="16">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
+      <c r="A14" t="s">
+        <v>246</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E14" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="16">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
+      <c r="A15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="16">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="2:4" ht="16">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="2:4" ht="16">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="2:4" ht="16">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="2:4" ht="16">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="2:4" ht="16">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="2:4" ht="16">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="2:4" ht="16">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="2:4" ht="16">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="2:4" ht="16">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
+      <c r="A16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16">
+      <c r="A17" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16">
+      <c r="A18" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16">
+      <c r="A19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16">
+      <c r="A20" t="s">
+        <v>258</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16">
+      <c r="A21" t="s">
+        <v>260</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16">
+      <c r="A22" t="s">
+        <v>262</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="E22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16">
+      <c r="A23" t="s">
+        <v>264</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16">
+      <c r="A25" t="s">
+        <v>268</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -2619,10 +3103,13 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16">
       <c r="A1" t="s">
@@ -2691,7 +3178,7 @@
         <v>80</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16">
@@ -2699,109 +3186,280 @@
         <v>146</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>211</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
+      <c r="A7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="16">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
+      <c r="A8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="16">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
+      <c r="A9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="16">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
+      <c r="A10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="16">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
+      <c r="A11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="16">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="A12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="16">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
+      <c r="A13" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="16">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
+      <c r="A14" t="s">
+        <v>246</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="16">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
+      <c r="A15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="16">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="2:4" ht="16">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="2:4" ht="16">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="2:4" ht="16">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="2:4" ht="16">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="2:4" ht="16">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="2:4" ht="16">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="2:4" ht="16">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="2:4" ht="16">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="2:4" ht="16">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
+      <c r="A16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16">
+      <c r="A17" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16">
+      <c r="A18" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16">
+      <c r="A19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16">
+      <c r="A20" t="s">
+        <v>258</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16">
+      <c r="A21" t="s">
+        <v>260</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16">
+      <c r="A22" t="s">
+        <v>262</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16">
+      <c r="A23" t="s">
+        <v>264</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16">
+      <c r="A25" t="s">
+        <v>268</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>231</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -2893,13 +3551,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E4" s="7">
         <v>0.03</v>
@@ -3110,13 +3768,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E4" s="7">
         <v>0.03</v>
@@ -3324,7 +3982,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3365,7 +4023,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3406,7 +4064,7 @@
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3447,7 +4105,7 @@
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3488,7 +4146,7 @@
         <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3571,13 +4229,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E4" s="7">
         <v>0</v>
@@ -3811,10 +4469,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>10</v>
@@ -3825,13 +4483,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>182</v>
       </c>
       <c r="E2" s="4">
         <v>532</v>
@@ -3848,13 +4506,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>184</v>
       </c>
       <c r="E3" s="4">
         <v>0</v>
@@ -3871,13 +4529,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>210</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
@@ -3919,13 +4577,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>186</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3933,16 +4591,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F2" s="2">
         <v>1.0000000000000001E-5</v>
@@ -3956,16 +4614,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>191</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F3" s="2">
         <v>2.0000000000000002E-5</v>
@@ -3979,16 +4637,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F4" s="2">
         <v>3.0000000000000001E-5</v>
@@ -4002,16 +4660,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F5" s="2">
         <v>4.0000000000000003E-5</v>
@@ -4058,22 +4716,22 @@
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I1" t="s">
         <v>45</v>
       </c>
       <c r="J1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" t="s">
         <v>170</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>171</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>172</v>
-      </c>
-      <c r="M1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -4081,13 +4739,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E2" s="3">
         <v>2</v>
@@ -4122,13 +4780,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -4163,13 +4821,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
@@ -4204,13 +4862,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E5" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
Minor change on pjm5bus_demo cost data
</commit_message>
<xml_diff>
--- a/ams/cases/5bus/pjm5bus_demo.xlsx
+++ b/ams/cases/5bus/pjm5bus_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/ams/ams/cases/5bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0074CA8-8290-5D4A-B617-D0C46F8D4279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B72769-B3A3-DF47-8CEB-42612E13A891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="21180" windowWidth="30240" windowHeight="18960" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30240" yWindow="21180" windowWidth="30240" windowHeight="18960" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -1677,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A0BCC1-5090-3645-97C9-41B78CF5D933}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="188" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.14499999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1782,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1817,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -5434,7 +5434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD37CC2-7295-9745-AE86-E7562082AFC8}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="240" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="240" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>

</xml_diff>